<commit_message>
generate create table sql and primary key
</commit_message>
<xml_diff>
--- a/TableSchema.xlsx
+++ b/TableSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CreateTableFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB543946-F2D0-42CD-92C2-A17799983CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E633C8-7F61-410C-ADC7-7593214B1415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t>Table Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TEST_SCHEMA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>測試註解</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BBB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>測試名稱1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -103,10 +95,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>VARCHA2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>50</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -184,6 +172,30 @@
   </si>
   <si>
     <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APUSER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16,2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -722,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -747,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -756,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>5</v>
@@ -823,18 +835,18 @@
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -852,23 +864,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -884,23 +896,23 @@
     </row>
     <row r="4" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -913,25 +925,25 @@
     </row>
     <row r="5" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -944,22 +956,22 @@
     </row>
     <row r="6" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -973,24 +985,24 @@
     </row>
     <row r="7" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -1004,18 +1016,20 @@
     </row>
     <row r="8" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+      <c r="H8" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="I8" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -1031,29 +1045,29 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>

</xml_diff>

<commit_message>
refactor to module in create table sql function
</commit_message>
<xml_diff>
--- a/TableSchema.xlsx
+++ b/TableSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CreateTableFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E633C8-7F61-410C-ADC7-7593214B1415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F3EC4-4579-49CB-AED7-4586B8B7A4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
   <si>
     <t>Table Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>測試名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TEST_NAME1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,6 +192,10 @@
   </si>
   <si>
     <t>16,2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試名稱0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -768,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>5</v>
@@ -835,23 +835,27 @@
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -867,20 +871,20 @@
         <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -896,23 +900,23 @@
     </row>
     <row r="4" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -925,25 +929,25 @@
     </row>
     <row r="5" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -956,25 +960,27 @@
     </row>
     <row r="6" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -985,27 +991,29 @@
     </row>
     <row r="7" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1016,26 +1024,28 @@
     </row>
     <row r="8" spans="1:20" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1045,29 +1055,29 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>

</xml_diff>

<commit_message>
use enum store data location in excel
</commit_message>
<xml_diff>
--- a/TableSchema.xlsx
+++ b/TableSchema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\CreateTableFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F3EC4-4579-49CB-AED7-4586B8B7A4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC20F07-6425-490E-B49E-BF11EEFB018A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,7 +735,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>

</xml_diff>